<commit_message>
implemented the usb-copy function (firs_test)
</commit_message>
<xml_diff>
--- a/presets/presets.xlsx
+++ b/presets/presets.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>10,10,15,20</t>
+  </si>
+  <si>
+    <t>Comosite #1</t>
+  </si>
+  <si>
+    <t>50-90</t>
+  </si>
+  <si>
+    <t>50,70,90</t>
   </si>
 </sst>
 </file>
@@ -691,7 +700,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -702,6 +711,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1041,13 +1051,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.6" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.6" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="16.6607142857143" customWidth="1"/>
     <col min="2" max="2" width="20.6607142857143" customWidth="1"/>
@@ -1096,6 +1106,20 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4">
+        <v>60120120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>